<commit_message>
Snapshot. Data prep mostly done. TOC in place.
</commit_message>
<xml_diff>
--- a/Submissions/UWKT3_Submissions.xlsx
+++ b/Submissions/UWKT3_Submissions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="30940" yWindow="580" windowWidth="18500" windowHeight="16040"/>
+    <workbookView xWindow="280" yWindow="11180" windowWidth="18500" windowHeight="16040"/>
   </bookViews>
   <sheets>
     <sheet name="Submissions" sheetId="3" r:id="rId1"/>
@@ -332,7 +332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -357,6 +357,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -567,7 +573,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="176">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1007,7 +1013,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1017,8 +1023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1134,7 +1140,7 @@
       <c r="E7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="15">
         <v>0.59641999999999995</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -1230,7 +1236,7 @@
       <c r="E11" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="15">
         <v>0.62834999999999996</v>
       </c>
       <c r="G11" s="10" t="s">

</xml_diff>

<commit_message>
Report RMarkdown, supporting files, and PDF as sent out to team as first rough ddraft.
</commit_message>
<xml_diff>
--- a/Submissions/UWKT3_Submissions.xlsx
+++ b/Submissions/UWKT3_Submissions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="11180" windowWidth="18500" windowHeight="16040"/>
+    <workbookView xWindow="26980" yWindow="2080" windowWidth="18500" windowHeight="18320"/>
   </bookViews>
   <sheets>
     <sheet name="Submissions" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
   <si>
     <t>Full</t>
   </si>
@@ -284,6 +284,21 @@
   </si>
   <si>
     <t>Submission_71862_0602_AE</t>
+  </si>
+  <si>
+    <t>test0528JS_WekaClassified.csv</t>
+  </si>
+  <si>
+    <t>Reproduced #7 above in R Markdown.</t>
+  </si>
+  <si>
+    <t>Attempted to reproduce #13 above in R Markdown.</t>
+  </si>
+  <si>
+    <t>Sanity check: re-submitted Andy's csv file from #13 above - not reproduced from Kaggle datasets in R.</t>
+  </si>
+  <si>
+    <t>Reproduced #13 above in R Markdown.</t>
   </si>
 </sst>
 </file>
@@ -294,9 +309,16 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -375,183 +397,183 @@
   </borders>
   <cellStyleXfs count="176">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -560,20 +582,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="176">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1021,10 +1053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1044,7 +1076,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15">
-      <c r="A3" t="s">
+      <c r="A3" s="21" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="7" t="s">
@@ -1140,7 +1172,7 @@
       <c r="E7" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="20">
         <v>0.59641999999999995</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -1332,7 +1364,7 @@
       <c r="E15" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="20">
         <v>0.66366999999999998</v>
       </c>
       <c r="G15" s="10" t="s">
@@ -1392,36 +1424,266 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="9"/>
-      <c r="G18" s="10"/>
+      <c r="B18" s="7">
+        <v>42159</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.61406000000000005</v>
+      </c>
+      <c r="G18" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="29" customHeight="1">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="10"/>
+      <c r="B19" s="7">
+        <v>42159</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="9">
+        <v>0.57096000000000002</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="29" customHeight="1">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="10"/>
+      <c r="B20" s="7">
+        <v>42159</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.71862000000000004</v>
+      </c>
+      <c r="G20" s="17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="29" customHeight="1">
+      <c r="A21" s="16">
+        <v>17</v>
+      </c>
+      <c r="B21" s="18">
+        <v>42159</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="19">
+        <v>0.71863999999999995</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="29" customHeight="1">
+      <c r="A22" s="16"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="17"/>
+    </row>
+    <row r="23" spans="1:7" ht="29" customHeight="1">
+      <c r="A23" s="16"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="17"/>
+    </row>
+    <row r="24" spans="1:7" ht="29" customHeight="1">
+      <c r="A24" s="16"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="17"/>
+    </row>
+    <row r="25" spans="1:7" ht="29" customHeight="1">
+      <c r="A25" s="16"/>
+      <c r="B25" s="18"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="17"/>
+    </row>
+    <row r="26" spans="1:7" ht="29" customHeight="1">
+      <c r="A26" s="16"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="17"/>
+    </row>
+    <row r="27" spans="1:7" ht="29" customHeight="1">
+      <c r="A27" s="16"/>
+      <c r="B27" s="18"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="17"/>
+    </row>
+    <row r="28" spans="1:7" ht="29" customHeight="1">
+      <c r="A28" s="16"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="17"/>
+    </row>
+    <row r="29" spans="1:7" ht="29" customHeight="1">
+      <c r="A29" s="16"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="17"/>
+    </row>
+    <row r="30" spans="1:7" ht="29" customHeight="1">
+      <c r="A30" s="16"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="16"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="17"/>
+    </row>
+    <row r="31" spans="1:7" ht="29" customHeight="1">
+      <c r="A31" s="16"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="16"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="17"/>
+    </row>
+    <row r="32" spans="1:7" ht="29" customHeight="1">
+      <c r="A32" s="16"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="17"/>
+    </row>
+    <row r="33" spans="1:7" ht="29" customHeight="1">
+      <c r="A33" s="16"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="17"/>
+    </row>
+    <row r="34" spans="1:7" ht="29" customHeight="1">
+      <c r="A34" s="16"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="17"/>
+    </row>
+    <row r="35" spans="1:7" ht="29" customHeight="1">
+      <c r="A35" s="16"/>
+      <c r="B35" s="18"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="17"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="17"/>
+    </row>
+    <row r="36" spans="1:7" ht="29" customHeight="1">
+      <c r="A36" s="16"/>
+      <c r="B36" s="18"/>
+      <c r="C36" s="16"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="17"/>
+    </row>
+    <row r="37" spans="1:7" ht="29" customHeight="1">
+      <c r="A37" s="16"/>
+      <c r="B37" s="18"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="17"/>
+    </row>
+    <row r="38" spans="1:7" ht="29" customHeight="1">
+      <c r="A38" s="16"/>
+      <c r="B38" s="18"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="17"/>
+    </row>
+    <row r="39" spans="1:7" ht="29" customHeight="1">
+      <c r="A39" s="16"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="16"/>
+      <c r="D39" s="17"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="17"/>
+    </row>
+    <row r="40" spans="1:7" ht="29" customHeight="1">
+      <c r="A40" s="16"/>
+      <c r="B40" s="18"/>
+      <c r="C40" s="16"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Submissions thru 1PM on 6-Jun-2015.
</commit_message>
<xml_diff>
--- a/Submissions/UWKT3_Submissions.xlsx
+++ b/Submissions/UWKT3_Submissions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26980" yWindow="2080" windowWidth="18500" windowHeight="18320"/>
+    <workbookView xWindow="25220" yWindow="2560" windowWidth="22060" windowHeight="22140"/>
   </bookViews>
   <sheets>
     <sheet name="Submissions" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="105">
   <si>
     <t>Full</t>
   </si>
@@ -283,22 +283,58 @@
     <t>Andy Ewing -- This submission uses BayHarborButcher's modification of mlandry's logistic regression. This uses a generalized additive model with week number instead of month and lat/long instead of block. I added average temp and average wind speed.</t>
   </si>
   <si>
-    <t>Submission_71862_0602_AE</t>
-  </si>
-  <si>
     <t>test0528JS_WekaClassified.csv</t>
   </si>
   <si>
-    <t>Reproduced #7 above in R Markdown.</t>
-  </si>
-  <si>
     <t>Attempted to reproduce #13 above in R Markdown.</t>
   </si>
   <si>
     <t>Sanity check: re-submitted Andy's csv file from #13 above - not reproduced from Kaggle datasets in R.</t>
   </si>
   <si>
-    <t>Reproduced #13 above in R Markdown.</t>
+    <t xml:space="preserve"> = Best Score</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = Reproduced from Kaggle datasets using R.</t>
+  </si>
+  <si>
+    <t>Reproduced #13 above in R Markdown. Both data preparation and modeling.</t>
+  </si>
+  <si>
+    <t>Reproduced #7 above in R Markdown. Just "golden" ARFF train and test datasets. Modeling done in Weka.</t>
+  </si>
+  <si>
+    <t>Submission_0602_AE_71862</t>
+  </si>
+  <si>
+    <t>Submit?</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Greg Hogue</t>
+  </si>
+  <si>
+    <t>WNV Submission.csv</t>
+  </si>
+  <si>
+    <t>AssocitedSubmissionUWKT3Russell.csv</t>
+  </si>
+  <si>
+    <t>WNV Submission 2.csv</t>
+  </si>
+  <si>
+    <t>Combination of naïve and associated learning techniques.</t>
+  </si>
+  <si>
+    <t>(Try 2) Using primarily weather and positional data (ignored the spray data as being incomplete), I converted the weather data into aggregates of weather data between the date the trap was checked and the date it was checked before. Using Weka, I applied SMOTE to even out the "Y"s from the "N"s, then used a Naive-Bayes tree on the features week-of-year, longitude, max temp, avg wetbulb, and avg resultspeed.</t>
+  </si>
+  <si>
+    <t>combines new associated rules with the previous naïve approach. The new rules focus on traps that have never had a WNV positive finding.</t>
+  </si>
+  <si>
+    <t>Using primarily weather and positional data (ignored the spray data as being incomplete), I converted the weather data into aggregates of weather data between the date the trap was checked and the date it was checked before. Using Weka, I applied SMOTE to even out the "Y"s from the "N"s, then used a Naive-Bayes tree on the features week-of-year, longitude, max temp, avg wetbulb, and avg resultspeed.</t>
   </si>
 </sst>
 </file>
@@ -309,7 +345,7 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,8 +389,14 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -385,6 +427,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -573,7 +621,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -606,6 +654,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="176">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1053,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1157,7 +1211,7 @@
     </row>
     <row r="7" spans="1:7" ht="29" customHeight="1">
       <c r="A7">
-        <f t="shared" ref="A7:A20" si="0">A6+1</f>
+        <f t="shared" ref="A7:A27" si="0">A6+1</f>
         <v>3</v>
       </c>
       <c r="B7" s="7">
@@ -1265,7 +1319,7 @@
       <c r="D11" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="16" t="s">
         <v>52</v>
       </c>
       <c r="F11" s="15">
@@ -1410,7 +1464,7 @@
         <v>85</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="F17" s="15">
         <v>0.71862000000000004</v>
@@ -1431,7 +1485,7 @@
         <v>82</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E18" s="16" t="s">
         <v>53</v>
@@ -1440,7 +1494,7 @@
         <v>0.61406000000000005</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="29" customHeight="1">
@@ -1464,7 +1518,7 @@
         <v>0.57096000000000002</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="29" customHeight="1">
@@ -1488,11 +1542,12 @@
         <v>0.71862000000000004</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="29" customHeight="1">
-      <c r="A21" s="16">
+      <c r="A21">
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B21" s="18">
@@ -1515,43 +1570,98 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="29" customHeight="1">
-      <c r="A22" s="16"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="17"/>
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B22" s="18">
+        <v>42160</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="17" t="s">
+        <v>98</v>
+      </c>
       <c r="E22" s="16"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="17"/>
+      <c r="F22" s="19">
+        <v>0.49978</v>
+      </c>
+      <c r="G22" s="17" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="29" customHeight="1">
-      <c r="A23" s="16"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="17"/>
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B23" s="18">
+        <v>42160</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>99</v>
+      </c>
       <c r="E23" s="16"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="17"/>
+      <c r="F23" s="19">
+        <v>0.66527999999999998</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="24" spans="1:7" ht="29" customHeight="1">
-      <c r="A24" s="16"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B24" s="18">
+        <v>42161</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="E24" s="16"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="17"/>
+      <c r="F24" s="19">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="29" customHeight="1">
-      <c r="A25" s="16"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B25" s="18">
+        <v>42161</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>99</v>
+      </c>
       <c r="E25" s="16"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="17"/>
+      <c r="F25" s="19">
+        <v>0.66891</v>
+      </c>
+      <c r="G25" s="17" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="29" customHeight="1">
-      <c r="A26" s="16"/>
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
       <c r="B26" s="18"/>
       <c r="C26" s="16"/>
       <c r="D26" s="17"/>
@@ -1560,7 +1670,10 @@
       <c r="G26" s="17"/>
     </row>
     <row r="27" spans="1:7" ht="29" customHeight="1">
-      <c r="A27" s="16"/>
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
       <c r="B27" s="18"/>
       <c r="C27" s="16"/>
       <c r="D27" s="17"/>
@@ -1587,8 +1700,10 @@
       <c r="G29" s="17"/>
     </row>
     <row r="30" spans="1:7" ht="29" customHeight="1">
-      <c r="A30" s="16"/>
-      <c r="B30" s="18"/>
+      <c r="A30" s="22"/>
+      <c r="B30" s="24" t="s">
+        <v>90</v>
+      </c>
       <c r="C30" s="16"/>
       <c r="D30" s="17"/>
       <c r="E30" s="16"/>
@@ -1596,8 +1711,10 @@
       <c r="G30" s="17"/>
     </row>
     <row r="31" spans="1:7" ht="29" customHeight="1">
-      <c r="A31" s="16"/>
-      <c r="B31" s="18"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="24" t="s">
+        <v>91</v>
+      </c>
       <c r="C31" s="16"/>
       <c r="D31" s="17"/>
       <c r="E31" s="16"/>
@@ -1684,6 +1801,69 @@
       <c r="E40" s="16"/>
       <c r="F40" s="19"/>
       <c r="G40" s="17"/>
+    </row>
+    <row r="41" spans="1:7" ht="29" customHeight="1">
+      <c r="A41" s="16"/>
+      <c r="B41" s="18"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="16"/>
+      <c r="F41" s="19"/>
+      <c r="G41" s="17"/>
+    </row>
+    <row r="42" spans="1:7" ht="29" customHeight="1">
+      <c r="A42" s="16"/>
+      <c r="B42" s="18"/>
+      <c r="C42" s="16"/>
+      <c r="D42" s="17"/>
+      <c r="E42" s="16"/>
+      <c r="F42" s="19"/>
+      <c r="G42" s="17"/>
+    </row>
+    <row r="43" spans="1:7" ht="29" customHeight="1">
+      <c r="A43" s="16"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="16"/>
+      <c r="D43" s="17"/>
+      <c r="E43" s="16"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="17"/>
+    </row>
+    <row r="44" spans="1:7" ht="29" customHeight="1">
+      <c r="A44" s="16"/>
+      <c r="B44" s="18"/>
+      <c r="C44" s="16"/>
+      <c r="D44" s="17"/>
+      <c r="E44" s="16"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="17"/>
+    </row>
+    <row r="45" spans="1:7" ht="29" customHeight="1">
+      <c r="A45" s="16"/>
+      <c r="B45" s="18"/>
+      <c r="C45" s="16"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="19"/>
+      <c r="G45" s="17"/>
+    </row>
+    <row r="46" spans="1:7" ht="29" customHeight="1">
+      <c r="A46" s="16"/>
+      <c r="B46" s="18"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="17"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="19"/>
+      <c r="G46" s="17"/>
+    </row>
+    <row r="47" spans="1:7" ht="29" customHeight="1">
+      <c r="A47" s="16"/>
+      <c r="B47" s="18"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="17"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1701,7 +1881,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1732,6 +1912,9 @@
       <c r="D4" t="s">
         <v>30</v>
       </c>
+      <c r="E4" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="1" t="s">
@@ -1746,6 +1929,7 @@
       <c r="D6" t="s">
         <v>31</v>
       </c>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
@@ -1760,6 +1944,9 @@
       <c r="D7" t="s">
         <v>32</v>
       </c>
+      <c r="E7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="1" t="s">
@@ -1774,6 +1961,7 @@
       <c r="D8" t="s">
         <v>33</v>
       </c>
+      <c r="E8" s="25"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="1" t="s">
@@ -1788,6 +1976,9 @@
       <c r="D9" t="s">
         <v>34</v>
       </c>
+      <c r="E9" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="11" t="s">
@@ -1819,6 +2010,9 @@
       <c r="D11" t="s">
         <v>36</v>
       </c>
+      <c r="E11" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="1" t="s">
@@ -1833,6 +2027,7 @@
       <c r="D12" t="s">
         <v>37</v>
       </c>
+      <c r="E12" s="25"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
@@ -1847,6 +2042,9 @@
       <c r="D13" t="s">
         <v>38</v>
       </c>
+      <c r="E13" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
@@ -1860,6 +2058,9 @@
       </c>
       <c r="D14" t="s">
         <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version sent out to team for final review on Monday June 8th.
</commit_message>
<xml_diff>
--- a/Submissions/UWKT3_Submissions.xlsx
+++ b/Submissions/UWKT3_Submissions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25220" yWindow="2560" windowWidth="22060" windowHeight="22140" activeTab="1"/>
+    <workbookView xWindow="25140" yWindow="1200" windowWidth="22060" windowHeight="22140"/>
   </bookViews>
   <sheets>
     <sheet name="Submissions" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="123">
   <si>
     <t>Full</t>
   </si>
@@ -295,9 +295,6 @@
     <t xml:space="preserve"> = Best Score</t>
   </si>
   <si>
-    <t xml:space="preserve"> = Reproduced from Kaggle datasets using R.</t>
-  </si>
-  <si>
     <t>Reproduced #13 above in R Markdown. Both data preparation and modeling.</t>
   </si>
   <si>
@@ -335,6 +332,75 @@
   </si>
   <si>
     <t>Using primarily weather and positional data (ignored the spray data as being incomplete), I converted the weather data into aggregates of weather data between the date the trap was checked and the date it was checked before. Using Weka, I applied SMOTE to even out the "Y"s from the "N"s, then used a Naive-Bayes tree on the features week-of-year, longitude, max temp, avg wetbulb, and avg resultspeed.</t>
+  </si>
+  <si>
+    <t>Beth Britt</t>
+  </si>
+  <si>
+    <t>BBSubmissions.csv</t>
+  </si>
+  <si>
+    <t>Decision tree and bagging.</t>
+  </si>
+  <si>
+    <t>Further refinement of associated learning rules.</t>
+  </si>
+  <si>
+    <t>WNV_RF_LQ.csv</t>
+  </si>
+  <si>
+    <t>Submission_0607_BB.csv</t>
+  </si>
+  <si>
+    <t>GPH Submission 3.csv</t>
+  </si>
+  <si>
+    <t>Using same data as before, I broke it up into four categories: each of the 3 most abundant species and an 'other' category that would all be forecast to zero. Used a random forest for each of the groups to arrive at forecast.</t>
+  </si>
+  <si>
+    <t>GPH Submission 4.csv</t>
+  </si>
+  <si>
+    <t>Started with new set of data having added back a bunch I had removed earlier.  Ran a naive-bayes decision tree...</t>
+  </si>
+  <si>
+    <r>
+      <t>Trained by RandomForest, but keep the original possibilities instead of converted to 0 and 1 as the prediction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Submission_72228_0607_LQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> = Reproduced in team report from Kaggle datasets. Input to Weka modeling, or modeling in R.</t>
+  </si>
+  <si>
+    <t>GPH Submission 5.csv</t>
+  </si>
+  <si>
+    <t>Same model and data as submission 4, however results for submission 4 may have been out of order. Attempting to correct that...</t>
+  </si>
+  <si>
+    <t>Jim Stearns, repro work of Linghua</t>
+  </si>
+  <si>
+    <t>Same script as June 7 submission of Linghua (#24).</t>
+  </si>
+  <si>
+    <t>wNileVirusRF.csv</t>
+  </si>
+  <si>
+    <t>Submission_73115_0608_LQJS</t>
   </si>
 </sst>
 </file>
@@ -345,9 +411,23 @@
     <numFmt numFmtId="164" formatCode="0.00000"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -393,6 +473,13 @@
       <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -443,185 +530,189 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="176">
+  <cellStyleXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -630,38 +721,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="176">
+  <cellStyles count="180">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -752,6 +875,8 @@
     <cellStyle name="Followed Hyperlink" xfId="173" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -837,6 +962,8 @@
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1107,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1118,752 +1245,879 @@
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="2" width="12.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.5" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.5" customWidth="1"/>
     <col min="6" max="6" width="11" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="50.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23">
       <c r="B1" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15">
-      <c r="A3" s="21" t="s">
+      <c r="G1" s="38"/>
+    </row>
+    <row r="2" spans="1:7" ht="23">
+      <c r="B2" s="6"/>
+      <c r="G2" s="38"/>
+    </row>
+    <row r="3" spans="1:7" ht="18">
+      <c r="A3" s="19"/>
+      <c r="B3" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="38"/>
+    </row>
+    <row r="4" spans="1:7" ht="18">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="G4" s="38"/>
+    </row>
+    <row r="5" spans="1:7" ht="23">
+      <c r="B5" s="6"/>
+      <c r="G5" s="38"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="G6" s="38"/>
+    </row>
+    <row r="7" spans="1:7" ht="15">
+      <c r="A7" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E7" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F7" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="G7" s="38" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15">
-      <c r="B4" s="7" t="s">
+    <row r="8" spans="1:7" ht="15">
+      <c r="B8" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" spans="1:7" ht="29" customHeight="1">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="7">
-        <v>42136</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="29" customHeight="1">
-      <c r="A6">
-        <f>A5+1</f>
-        <v>2</v>
-      </c>
-      <c r="B6" s="7">
-        <v>42141</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="29" customHeight="1">
-      <c r="A7">
-        <f t="shared" ref="A7:A27" si="0">A6+1</f>
-        <v>3</v>
-      </c>
-      <c r="B7" s="7">
-        <v>42141</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F7" s="20">
-        <v>0.59641999999999995</v>
-      </c>
-      <c r="G7" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="29" customHeight="1">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B8" s="7">
-        <v>42151</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="9">
-        <v>0.50312000000000001</v>
-      </c>
-      <c r="G8" s="10" t="s">
-        <v>63</v>
-      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="38"/>
     </row>
     <row r="9" spans="1:7" ht="29" customHeight="1">
       <c r="A9">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B9" s="7">
-        <v>42151</v>
+        <v>42136</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F9" s="9">
-        <v>0.61289000000000005</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>65</v>
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="38" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" customHeight="1">
       <c r="A10">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f>A9+1</f>
+        <v>2</v>
       </c>
       <c r="B10" s="7">
-        <v>42152</v>
+        <v>42141</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F10" s="9">
-        <v>0.49206</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>78</v>
+        <v>0.5</v>
+      </c>
+      <c r="G10" s="38" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="29" customHeight="1">
       <c r="A11">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f t="shared" ref="A11:A34" si="0">A10+1</f>
+        <v>3</v>
       </c>
       <c r="B11" s="7">
-        <v>42152</v>
+        <v>42141</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="15">
-        <v>0.62834999999999996</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>66</v>
+        <v>57</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F11" s="17">
+        <v>0.59641999999999995</v>
+      </c>
+      <c r="G11" s="38" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" customHeight="1">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B12" s="7">
-        <v>42152</v>
+        <v>42151</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>82</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>53</v>
       </c>
       <c r="F12" s="9">
-        <v>0.51902000000000004</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>67</v>
+        <v>0.50312000000000001</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" customHeight="1">
       <c r="A13">
-        <f>A12+1</f>
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="B13" s="7">
-        <v>42156</v>
+        <v>42151</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F13" s="9">
-        <v>0.49944</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>69</v>
+        <v>0.61289000000000005</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="29" customHeight="1">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B14" s="7">
-        <v>42156</v>
+        <v>42152</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>53</v>
       </c>
       <c r="F14" s="9">
-        <v>0.49925000000000003</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>71</v>
+        <v>0.49206</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="29" customHeight="1">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B15" s="7">
-        <v>42156</v>
+        <v>42152</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="20">
-        <v>0.66366999999999998</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>74</v>
+        <v>49</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0.62834999999999996</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="29" customHeight="1">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B16" s="7">
-        <v>42157</v>
+        <v>42152</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>76</v>
+        <v>53</v>
       </c>
       <c r="F16" s="9">
-        <v>0.67093999999999998</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" ht="75" customHeight="1">
+        <v>0.51902000000000004</v>
+      </c>
+      <c r="G16" s="38" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="29" customHeight="1">
       <c r="A17">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B17" s="12">
-        <v>42157</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="F17" s="15">
-        <v>0.71862000000000004</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>86</v>
+        <f>A16+1</f>
+        <v>9</v>
+      </c>
+      <c r="B17" s="7">
+        <v>42156</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="9">
+        <v>0.49944</v>
+      </c>
+      <c r="G17" s="38" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="29" customHeight="1">
       <c r="A18">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B18" s="7">
-        <v>42159</v>
-      </c>
-      <c r="C18" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" s="16" t="s">
+        <v>42156</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>53</v>
       </c>
       <c r="F18" s="9">
-        <v>0.61406000000000005</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>93</v>
+        <v>0.49925000000000003</v>
+      </c>
+      <c r="G18" s="38" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="29" customHeight="1">
       <c r="A19">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B19" s="7">
-        <v>42159</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="9">
-        <v>0.57096000000000002</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>88</v>
+        <v>42156</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F19" s="17">
+        <v>0.66366999999999998</v>
+      </c>
+      <c r="G19" s="38" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="29" customHeight="1">
       <c r="A20">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B20" s="7">
-        <v>42159</v>
-      </c>
-      <c r="C20" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="17" t="s">
+        <v>42157</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.67093999999999998</v>
+      </c>
+      <c r="G20" s="38" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="1" customFormat="1" ht="75" customHeight="1">
+      <c r="A21" s="1">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B21" s="30">
+        <v>42157</v>
+      </c>
+      <c r="C21" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="9">
+      <c r="E21" s="31" t="s">
+        <v>93</v>
+      </c>
+      <c r="F21" s="12">
         <v>0.71862000000000004</v>
       </c>
-      <c r="G20" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="29" customHeight="1">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B21" s="18">
-        <v>42159</v>
-      </c>
-      <c r="C21" s="16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>85</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="19">
-        <v>0.71863999999999995</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>92</v>
+      <c r="G21" s="39" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="29" customHeight="1">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B22" s="18">
-        <v>42160</v>
-      </c>
-      <c r="C22" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="16"/>
-      <c r="F22" s="19">
-        <v>0.49978</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>104</v>
+        <v>14</v>
+      </c>
+      <c r="B22" s="7">
+        <v>42159</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.61406000000000005</v>
+      </c>
+      <c r="G22" s="38" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="29" customHeight="1">
       <c r="A23">
         <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B23" s="18">
-        <v>42160</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E23" s="16"/>
-      <c r="F23" s="19">
-        <v>0.66527999999999998</v>
-      </c>
-      <c r="G23" s="17" t="s">
-        <v>103</v>
+        <v>15</v>
+      </c>
+      <c r="B23" s="7">
+        <v>42159</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0.57096000000000002</v>
+      </c>
+      <c r="G23" s="38" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="29" customHeight="1">
       <c r="A24">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B24" s="18">
-        <v>42161</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="E24" s="16"/>
-      <c r="F24" s="19">
-        <v>0.54500000000000004</v>
-      </c>
-      <c r="G24" s="17" t="s">
-        <v>102</v>
+        <v>16</v>
+      </c>
+      <c r="B24" s="7">
+        <v>42159</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0.71862000000000004</v>
+      </c>
+      <c r="G24" s="38" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="29" customHeight="1">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B25" s="18">
-        <v>42161</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E25" s="16"/>
-      <c r="F25" s="19">
-        <v>0.66891</v>
-      </c>
-      <c r="G25" s="17" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="29" customHeight="1">
+        <v>17</v>
+      </c>
+      <c r="B25" s="15">
+        <v>42159</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="F25" s="16">
+        <v>0.71863999999999995</v>
+      </c>
+      <c r="G25" s="38" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="42" customHeight="1">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="17"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="17"/>
+        <v>18</v>
+      </c>
+      <c r="B26" s="15">
+        <v>42160</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E26" s="13"/>
+      <c r="F26" s="16">
+        <v>0.49978</v>
+      </c>
+      <c r="G26" s="38" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="29" customHeight="1">
       <c r="A27">
         <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B27" s="15">
+        <v>42160</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="16">
+        <v>0.66527999999999998</v>
+      </c>
+      <c r="G27" s="38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="29" customHeight="1">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B28" s="15">
+        <v>42161</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="13"/>
+      <c r="F28" s="16">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="G28" s="38" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="29" customHeight="1">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B29" s="15">
+        <v>42161</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="13"/>
+      <c r="F29" s="16">
+        <v>0.66891</v>
+      </c>
+      <c r="G29" s="38" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="29" customHeight="1">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B30" s="15">
+        <v>42161</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="16">
+        <v>0.54551000000000005</v>
+      </c>
+      <c r="G30" s="38" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="29" customHeight="1">
+      <c r="A31">
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B27" s="18"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="17"/>
-    </row>
-    <row r="28" spans="1:7" ht="29" customHeight="1">
-      <c r="A28" s="16"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="17"/>
-    </row>
-    <row r="29" spans="1:7" ht="29" customHeight="1">
-      <c r="A29" s="16"/>
-      <c r="B29" s="18"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="17"/>
-    </row>
-    <row r="30" spans="1:7" ht="29" customHeight="1">
-      <c r="A30" s="22"/>
-      <c r="B30" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="17"/>
-    </row>
-    <row r="31" spans="1:7" ht="29" customHeight="1">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="C31" s="16"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="17"/>
-    </row>
-    <row r="32" spans="1:7" ht="29" customHeight="1">
-      <c r="A32" s="16"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="17"/>
-    </row>
-    <row r="33" spans="1:7" ht="29" customHeight="1">
-      <c r="A33" s="16"/>
-      <c r="B33" s="18"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="17"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="17"/>
-    </row>
-    <row r="34" spans="1:7" ht="29" customHeight="1">
-      <c r="A34" s="16"/>
-      <c r="B34" s="18"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="17"/>
+      <c r="B31" s="15">
+        <v>42162</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="16">
+        <v>0.67693999999999999</v>
+      </c>
+      <c r="G31" s="38" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="25" customFormat="1" ht="29" customHeight="1">
+      <c r="A32" s="25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B32" s="26">
+        <v>42162</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="D32" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="29">
+        <v>0.72228000000000003</v>
+      </c>
+      <c r="G32" s="40" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="1" customFormat="1" ht="55" customHeight="1">
+      <c r="A33" s="1">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B33" s="33">
+        <v>42163</v>
+      </c>
+      <c r="C33" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="E33" s="34"/>
+      <c r="F33" s="35">
+        <v>0.55362</v>
+      </c>
+      <c r="G33" s="39" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" s="1" customFormat="1" ht="29" customHeight="1">
+      <c r="A34" s="1">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B34" s="33">
+        <v>42163</v>
+      </c>
+      <c r="C34" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="E34" s="34"/>
+      <c r="F34" s="35">
+        <v>0.49431999999999998</v>
+      </c>
+      <c r="G34" s="39" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="29" customHeight="1">
-      <c r="A35" s="16"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="17"/>
-    </row>
-    <row r="36" spans="1:7" ht="29" customHeight="1">
-      <c r="A36" s="16"/>
-      <c r="B36" s="18"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="17"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="17"/>
+      <c r="A35" s="13">
+        <v>27</v>
+      </c>
+      <c r="B35" s="15">
+        <v>42163</v>
+      </c>
+      <c r="C35" s="42" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>117</v>
+      </c>
+      <c r="E35" s="13"/>
+      <c r="F35" s="16">
+        <v>0.59286000000000005</v>
+      </c>
+      <c r="G35" s="38" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="43" customHeight="1">
+      <c r="A36">
+        <v>28</v>
+      </c>
+      <c r="B36" s="4">
+        <v>42163</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="D36" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="42" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" s="16">
+        <v>0.73114999999999997</v>
+      </c>
+      <c r="G36" s="43" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="37" spans="1:7" ht="29" customHeight="1">
-      <c r="A37" s="16"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="19"/>
-      <c r="G37" s="17"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="14"/>
     </row>
     <row r="38" spans="1:7" ht="29" customHeight="1">
-      <c r="A38" s="16"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="19"/>
-      <c r="G38" s="17"/>
+      <c r="A38" s="13"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="14"/>
     </row>
     <row r="39" spans="1:7" ht="29" customHeight="1">
-      <c r="A39" s="16"/>
-      <c r="B39" s="18"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="16"/>
-      <c r="F39" s="19"/>
-      <c r="G39" s="17"/>
+      <c r="A39" s="13"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="13"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="14"/>
     </row>
     <row r="40" spans="1:7" ht="29" customHeight="1">
-      <c r="A40" s="16"/>
-      <c r="B40" s="18"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="17"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="19"/>
-      <c r="G40" s="17"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="14"/>
     </row>
     <row r="41" spans="1:7" ht="29" customHeight="1">
-      <c r="A41" s="16"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="17"/>
-      <c r="E41" s="16"/>
-      <c r="F41" s="19"/>
-      <c r="G41" s="17"/>
+      <c r="A41" s="13"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="13"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="14"/>
     </row>
     <row r="42" spans="1:7" ht="29" customHeight="1">
-      <c r="A42" s="16"/>
-      <c r="B42" s="18"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="17"/>
-      <c r="E42" s="16"/>
-      <c r="F42" s="19"/>
-      <c r="G42" s="17"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="13"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="14"/>
     </row>
     <row r="43" spans="1:7" ht="29" customHeight="1">
-      <c r="A43" s="16"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="16"/>
-      <c r="F43" s="19"/>
-      <c r="G43" s="17"/>
+      <c r="A43" s="13"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="13"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="14"/>
     </row>
     <row r="44" spans="1:7" ht="29" customHeight="1">
-      <c r="A44" s="16"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="16"/>
-      <c r="F44" s="19"/>
-      <c r="G44" s="17"/>
+      <c r="A44" s="13"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="13"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="14"/>
     </row>
     <row r="45" spans="1:7" ht="29" customHeight="1">
-      <c r="A45" s="16"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="17"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="19"/>
-      <c r="G45" s="17"/>
+      <c r="A45" s="13"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="13"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="14"/>
     </row>
     <row r="46" spans="1:7" ht="29" customHeight="1">
-      <c r="A46" s="16"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="17"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="19"/>
-      <c r="G46" s="17"/>
+      <c r="A46" s="13"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="13"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="14"/>
     </row>
     <row r="47" spans="1:7" ht="29" customHeight="1">
-      <c r="A47" s="16"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="19"/>
-      <c r="G47" s="17"/>
+      <c r="A47" s="13"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="13"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="14"/>
+    </row>
+    <row r="48" spans="1:7" ht="29" customHeight="1">
+      <c r="A48" s="13"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="13"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="14"/>
+    </row>
+    <row r="49" spans="1:7" ht="29" customHeight="1">
+      <c r="A49" s="13"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="14"/>
+    </row>
+    <row r="50" spans="1:7" ht="29" customHeight="1">
+      <c r="A50" s="13"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="14"/>
+    </row>
+    <row r="51" spans="1:7" ht="29" customHeight="1">
+      <c r="A51" s="13"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="13"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="14"/>
+    </row>
+    <row r="52" spans="1:7" ht="29" customHeight="1">
+      <c r="A52" s="13"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="13"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="14"/>
+    </row>
+    <row r="53" spans="1:7" ht="29" customHeight="1">
+      <c r="A53" s="13"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1880,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1913,7 +2167,7 @@
         <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -1929,7 +2183,9 @@
       <c r="D6" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="1" t="s">
@@ -1945,7 +2201,7 @@
         <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1962,7 +2218,7 @@
         <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1979,7 +2235,7 @@
         <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2013,7 +2269,7 @@
         <v>36</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -2029,7 +2285,7 @@
       <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="25"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
@@ -2045,7 +2301,7 @@
         <v>38</v>
       </c>
       <c r="E13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2062,7 +2318,7 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
As submitted as final team report to UW PCE Catalyst Homework DropBox.
</commit_message>
<xml_diff>
--- a/Submissions/UWKT3_Submissions.xlsx
+++ b/Submissions/UWKT3_Submissions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25140" yWindow="1200" windowWidth="22060" windowHeight="22140"/>
+    <workbookView xWindow="29720" yWindow="11960" windowWidth="20100" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="Submissions" sheetId="3" r:id="rId1"/>
@@ -530,7 +530,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="180">
+  <cellStyleXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -706,6 +706,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -784,7 +790,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="180">
+  <cellStyles count="186">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -877,6 +883,9 @@
     <cellStyle name="Followed Hyperlink" xfId="175" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="177" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="179" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="181" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="183" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="185" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -964,6 +973,9 @@
     <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="176" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="178" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="180" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="182" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="184" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1236,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1766,7 +1778,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="29" customHeight="1">
+    <row r="28" spans="1:7" ht="102" customHeight="1">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>20</v>

</xml_diff>